<commit_message>
Added all schmatics about to change LDO 1 to buck
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="108" documentId="11_F25DC773A252ABDACC104874091948605ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E76645A-7568-4BC4-8B6A-6DC8862F285B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18765" yWindow="3285" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -290,6 +290,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -756,7 +760,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added logo and assigned parts
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/abinash1_ualberta_ca/Documents/Desktop/side/CAN-USB RF Module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="11_F25DC773A252ABDACC104874091948605ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BA957CC-5C82-4323-8AA2-C61E7080C17E}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="11_F25DC773A252ABDACC104874091948605ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{747B714C-1B97-4E5D-930D-238249E695AD}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4260" yWindow="0" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Part Purpose</t>
   </si>
@@ -214,13 +214,22 @@
   </si>
   <si>
     <t>AZ1117IH-5.0TRG1</t>
+  </si>
+  <si>
+    <t>Common cathode Shotkey</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/nexperia-usa-inc/BAT160C-115/1232113</t>
+  </si>
+  <si>
+    <t>BAT160C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +257,14 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -277,7 +294,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,6 +303,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,6 +783,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{F079C007-3EC1-4CD0-B63A-529386FE93DA}"/>
@@ -777,9 +808,10 @@
     <hyperlink ref="C10" r:id="rId10" xr:uid="{C7F9B4BB-0A1C-4AE1-95BC-B1C8EECD9AD7}"/>
     <hyperlink ref="C11" r:id="rId11" xr:uid="{2A55919A-EF1F-4422-8A7E-04750FD25E41}"/>
     <hyperlink ref="C9" r:id="rId12" xr:uid="{120BA7F7-B911-41AE-80A5-765B4F0151E4}"/>
+    <hyperlink ref="C2" r:id="rId13" xr:uid="{049E4839-68CF-45A6-B11E-7A08BBCBDFE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -838,22 +870,22 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>